<commit_message>
Corrected title for winner
</commit_message>
<xml_diff>
--- a/CompLaagRayon/files/template-excel-rk-25m1pijl-indiv.xlsx
+++ b/CompLaagRayon/files/template-excel-rk-25m1pijl-indiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\RK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116E59FB-8AF6-449C-B91C-EC14ABA55DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E766568-D01B-4226-8735-A5765C6DCC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="1410" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1065" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
@@ -1664,7 +1664,7 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="50" t="str">
-        <f t="shared" ref="R8:R31" si="2">IF(S8=$Y$5,"Bondskampioen",IF(S8=$Y$7,"2e plaats",IF(S8=$Y$8,"3e plaats","")))</f>
+        <f>IF(S8=$Y$5,"Rayonkampioen",IF(S8=$Y$7,"2e plaats",IF(S8=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S8" s="13">
@@ -1705,7 +1705,7 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S9=$Y$5,"Rayonkampioen",IF(S9=$Y$7,"2e plaats",IF(S9=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S9" s="13">
@@ -1739,7 +1739,7 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S10=$Y$5,"Rayonkampioen",IF(S10=$Y$7,"2e plaats",IF(S10=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S10" s="13">
@@ -1773,7 +1773,7 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S11=$Y$5,"Rayonkampioen",IF(S11=$Y$7,"2e plaats",IF(S11=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S11" s="13">
@@ -1807,7 +1807,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S12=$Y$5,"Rayonkampioen",IF(S12=$Y$7,"2e plaats",IF(S12=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S12" s="13">
@@ -1841,7 +1841,7 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S13=$Y$5,"Rayonkampioen",IF(S13=$Y$7,"2e plaats",IF(S13=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S13" s="13">
@@ -1875,7 +1875,7 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S14=$Y$5,"Rayonkampioen",IF(S14=$Y$7,"2e plaats",IF(S14=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S14" s="13">
@@ -1909,7 +1909,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S15=$Y$5,"Rayonkampioen",IF(S15=$Y$7,"2e plaats",IF(S15=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S15" s="13">
@@ -1943,7 +1943,7 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S16=$Y$5,"Rayonkampioen",IF(S16=$Y$7,"2e plaats",IF(S16=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S16" s="13">
@@ -1977,7 +1977,7 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S17=$Y$5,"Rayonkampioen",IF(S17=$Y$7,"2e plaats",IF(S17=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S17" s="13">
@@ -2011,7 +2011,7 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S18=$Y$5,"Rayonkampioen",IF(S18=$Y$7,"2e plaats",IF(S18=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S18" s="13">
@@ -2045,7 +2045,7 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S19=$Y$5,"Rayonkampioen",IF(S19=$Y$7,"2e plaats",IF(S19=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S19" s="13">
@@ -2079,7 +2079,7 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S20=$Y$5,"Rayonkampioen",IF(S20=$Y$7,"2e plaats",IF(S20=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S20" s="13">
@@ -2113,7 +2113,7 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S21=$Y$5,"Rayonkampioen",IF(S21=$Y$7,"2e plaats",IF(S21=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S21" s="13">
@@ -2147,7 +2147,7 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S22=$Y$5,"Rayonkampioen",IF(S22=$Y$7,"2e plaats",IF(S22=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S22" s="13">
@@ -2181,7 +2181,7 @@
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S23=$Y$5,"Rayonkampioen",IF(S23=$Y$7,"2e plaats",IF(S23=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S23" s="13">
@@ -2215,7 +2215,7 @@
       <c r="P24"/>
       <c r="Q24"/>
       <c r="R24" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S24=$Y$5,"Rayonkampioen",IF(S24=$Y$7,"2e plaats",IF(S24=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S24" s="13">
@@ -2249,7 +2249,7 @@
       <c r="P25"/>
       <c r="Q25"/>
       <c r="R25" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S25=$Y$5,"Rayonkampioen",IF(S25=$Y$7,"2e plaats",IF(S25=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S25" s="13">
@@ -2283,7 +2283,7 @@
       <c r="P26"/>
       <c r="Q26"/>
       <c r="R26" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S26=$Y$5,"Rayonkampioen",IF(S26=$Y$7,"2e plaats",IF(S26=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S26" s="13">
@@ -2317,7 +2317,7 @@
       <c r="P27"/>
       <c r="Q27"/>
       <c r="R27" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S27=$Y$5,"Rayonkampioen",IF(S27=$Y$7,"2e plaats",IF(S27=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S27" s="13">
@@ -2351,7 +2351,7 @@
       <c r="P28"/>
       <c r="Q28"/>
       <c r="R28" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S28=$Y$5,"Rayonkampioen",IF(S28=$Y$7,"2e plaats",IF(S28=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S28" s="13">
@@ -2385,7 +2385,7 @@
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S29=$Y$5,"Rayonkampioen",IF(S29=$Y$7,"2e plaats",IF(S29=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S29" s="13">
@@ -2419,7 +2419,7 @@
       <c r="P30"/>
       <c r="Q30"/>
       <c r="R30" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S30=$Y$5,"Rayonkampioen",IF(S30=$Y$7,"2e plaats",IF(S30=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S30" s="13">
@@ -2453,7 +2453,7 @@
       <c r="P31"/>
       <c r="Q31"/>
       <c r="R31" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(S31=$Y$5,"Rayonkampioen",IF(S31=$Y$7,"2e plaats",IF(S31=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S31" s="13">
@@ -2478,7 +2478,7 @@
       <c r="J32" s="62"/>
       <c r="K32" s="62"/>
       <c r="L32" s="69" t="str">
-        <f t="shared" ref="L32" si="3">IF(J32&lt;&gt;"",J32+K32,"")</f>
+        <f t="shared" ref="L32" si="2">IF(J32&lt;&gt;"",J32+K32,"")</f>
         <v/>
       </c>
       <c r="M32" s="62"/>

</xml_diff>

<commit_message>
Moved date to same cell as for Indoor
</commit_message>
<xml_diff>
--- a/CompLaagRayon/files/template-excel-rk-25m1pijl-indiv.xlsx
+++ b/CompLaagRayon/files/template-excel-rk-25m1pijl-indiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\RK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E766568-D01B-4226-8735-A5765C6DCC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5773B2E-FFFE-462D-8986-73332D388642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1065" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="690" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
@@ -471,7 +471,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -636,10 +636,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -1358,7 +1354,9 @@
   </sheetPr>
   <dimension ref="A1:Y252"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:R3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1386,7 +1384,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
+      <c r="A1" s="54"/>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -1411,61 +1409,61 @@
     <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
-      <c r="C2" s="81" t="str">
+      <c r="C2" s="80" t="str">
         <f>"Rayonkampioenschappen 25m1pijl &lt;seizoen&gt;, Rayon #, &lt;klasse&gt;"</f>
         <v>Rayonkampioenschappen 25m1pijl &lt;seizoen&gt;, Rayon #, &lt;klasse&gt;</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="83"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="82"/>
       <c r="S2" s="39"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="47"/>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="79"/>
+      <c r="E3" s="78"/>
       <c r="F3" s="42"/>
       <c r="G3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="86"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="79" t="s">
+      <c r="I3" s="85"/>
+      <c r="J3" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="88" t="s">
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
     </row>
     <row r="4" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="39"/>
@@ -1477,22 +1475,22 @@
       <c r="G4" s="43"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="87"/>
+      <c r="K4" s="86"/>
       <c r="L4" s="46"/>
-      <c r="M4" s="84" t="s">
+      <c r="M4" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="84"/>
+      <c r="N4" s="83"/>
       <c r="O4" s="22"/>
       <c r="P4" s="45"/>
       <c r="Q4" s="45"/>
       <c r="R4" s="51"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
       <c r="X4" s="53" t="s">
         <v>42</v>
       </c>
@@ -1502,10 +1500,10 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="85"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="48">
         <v>0</v>
       </c>
@@ -1548,7 +1546,7 @@
       <c r="R5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="76" t="s">
+      <c r="S5" s="75" t="s">
         <v>31</v>
       </c>
       <c r="T5" s="25" t="s">
@@ -1584,7 +1582,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="52"/>
-      <c r="S6" s="75" t="s">
+      <c r="S6" s="74" t="s">
         <v>55</v>
       </c>
       <c r="T6" s="25"/>
@@ -1615,17 +1613,14 @@
       <c r="I7" s="20"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="23" t="str">
-        <f t="shared" ref="L7:L31" si="0">IF(J7&lt;&gt;"",J7+K7,"")</f>
-        <v/>
-      </c>
+      <c r="L7" s="23"/>
       <c r="M7" s="23"/>
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="50" t="str">
-        <f>IF(S7=$Y$5,"Rayonkampioen",IF(S7=$Y$7,"2e plaats",IF(S7=$Y$8,"3e plaats","")))</f>
+        <f t="shared" ref="R7:R31" si="0">IF(S7=$Y$5,"Rayonkampioen",IF(S7=$Y$7,"2e plaats",IF(S7=$Y$8,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S7" s="13">
@@ -1654,17 +1649,14 @@
       <c r="I8" s="20"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="50" t="str">
-        <f>IF(S8=$Y$5,"Rayonkampioen",IF(S8=$Y$7,"2e plaats",IF(S8=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S8" s="13">
@@ -1695,17 +1687,14 @@
       <c r="I9" s="20"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="50" t="str">
-        <f>IF(S9=$Y$5,"Rayonkampioen",IF(S9=$Y$7,"2e plaats",IF(S9=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S9" s="13">
@@ -1730,7 +1719,7 @@
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>
       <c r="L10" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L7:L31" si="2">IF(J10&lt;&gt;"",J10+K10,"")</f>
         <v/>
       </c>
       <c r="M10" s="23"/>
@@ -1739,7 +1728,7 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="50" t="str">
-        <f>IF(S10=$Y$5,"Rayonkampioen",IF(S10=$Y$7,"2e plaats",IF(S10=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S10" s="13">
@@ -1764,7 +1753,7 @@
       <c r="J11" s="23"/>
       <c r="K11" s="23"/>
       <c r="L11" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M11" s="23"/>
@@ -1773,7 +1762,7 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="50" t="str">
-        <f>IF(S11=$Y$5,"Rayonkampioen",IF(S11=$Y$7,"2e plaats",IF(S11=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S11" s="13">
@@ -1798,7 +1787,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
       <c r="L12" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M12" s="23"/>
@@ -1807,7 +1796,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="50" t="str">
-        <f>IF(S12=$Y$5,"Rayonkampioen",IF(S12=$Y$7,"2e plaats",IF(S12=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S12" s="13">
@@ -1832,7 +1821,7 @@
       <c r="J13" s="23"/>
       <c r="K13" s="23"/>
       <c r="L13" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M13" s="23"/>
@@ -1841,7 +1830,7 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="50" t="str">
-        <f>IF(S13=$Y$5,"Rayonkampioen",IF(S13=$Y$7,"2e plaats",IF(S13=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S13" s="13">
@@ -1866,7 +1855,7 @@
       <c r="J14" s="23"/>
       <c r="K14" s="23"/>
       <c r="L14" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M14" s="23"/>
@@ -1875,7 +1864,7 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="50" t="str">
-        <f>IF(S14=$Y$5,"Rayonkampioen",IF(S14=$Y$7,"2e plaats",IF(S14=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S14" s="13">
@@ -1900,7 +1889,7 @@
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M15" s="23"/>
@@ -1909,7 +1898,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="50" t="str">
-        <f>IF(S15=$Y$5,"Rayonkampioen",IF(S15=$Y$7,"2e plaats",IF(S15=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S15" s="13">
@@ -1934,7 +1923,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M16" s="23"/>
@@ -1943,7 +1932,7 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="50" t="str">
-        <f>IF(S16=$Y$5,"Rayonkampioen",IF(S16=$Y$7,"2e plaats",IF(S16=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S16" s="13">
@@ -1968,7 +1957,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M17" s="23"/>
@@ -1977,7 +1966,7 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="50" t="str">
-        <f>IF(S17=$Y$5,"Rayonkampioen",IF(S17=$Y$7,"2e plaats",IF(S17=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S17" s="13">
@@ -2002,7 +1991,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M18" s="23"/>
@@ -2011,7 +2000,7 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="50" t="str">
-        <f>IF(S18=$Y$5,"Rayonkampioen",IF(S18=$Y$7,"2e plaats",IF(S18=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S18" s="13">
@@ -2036,7 +2025,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
       <c r="L19" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M19" s="23"/>
@@ -2045,7 +2034,7 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="50" t="str">
-        <f>IF(S19=$Y$5,"Rayonkampioen",IF(S19=$Y$7,"2e plaats",IF(S19=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S19" s="13">
@@ -2070,7 +2059,7 @@
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
       <c r="L20" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M20" s="23"/>
@@ -2079,7 +2068,7 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="50" t="str">
-        <f>IF(S20=$Y$5,"Rayonkampioen",IF(S20=$Y$7,"2e plaats",IF(S20=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S20" s="13">
@@ -2104,7 +2093,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
       <c r="L21" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M21" s="23"/>
@@ -2113,7 +2102,7 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="50" t="str">
-        <f>IF(S21=$Y$5,"Rayonkampioen",IF(S21=$Y$7,"2e plaats",IF(S21=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S21" s="13">
@@ -2138,7 +2127,7 @@
       <c r="J22" s="23"/>
       <c r="K22" s="23"/>
       <c r="L22" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M22" s="23"/>
@@ -2147,7 +2136,7 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="50" t="str">
-        <f>IF(S22=$Y$5,"Rayonkampioen",IF(S22=$Y$7,"2e plaats",IF(S22=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S22" s="13">
@@ -2172,7 +2161,7 @@
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
       <c r="L23" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M23" s="21"/>
@@ -2181,7 +2170,7 @@
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23" s="50" t="str">
-        <f>IF(S23=$Y$5,"Rayonkampioen",IF(S23=$Y$7,"2e plaats",IF(S23=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S23" s="13">
@@ -2206,7 +2195,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M24" s="21"/>
@@ -2215,7 +2204,7 @@
       <c r="P24"/>
       <c r="Q24"/>
       <c r="R24" s="50" t="str">
-        <f>IF(S24=$Y$5,"Rayonkampioen",IF(S24=$Y$7,"2e plaats",IF(S24=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S24" s="13">
@@ -2240,7 +2229,7 @@
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
       <c r="L25" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M25" s="21"/>
@@ -2249,7 +2238,7 @@
       <c r="P25"/>
       <c r="Q25"/>
       <c r="R25" s="50" t="str">
-        <f>IF(S25=$Y$5,"Rayonkampioen",IF(S25=$Y$7,"2e plaats",IF(S25=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S25" s="13">
@@ -2274,7 +2263,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
       <c r="L26" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M26" s="21"/>
@@ -2283,7 +2272,7 @@
       <c r="P26"/>
       <c r="Q26"/>
       <c r="R26" s="50" t="str">
-        <f>IF(S26=$Y$5,"Rayonkampioen",IF(S26=$Y$7,"2e plaats",IF(S26=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S26" s="13">
@@ -2308,7 +2297,7 @@
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
       <c r="L27" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M27" s="21"/>
@@ -2317,7 +2306,7 @@
       <c r="P27"/>
       <c r="Q27"/>
       <c r="R27" s="50" t="str">
-        <f>IF(S27=$Y$5,"Rayonkampioen",IF(S27=$Y$7,"2e plaats",IF(S27=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S27" s="13">
@@ -2342,7 +2331,7 @@
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M28" s="21"/>
@@ -2351,7 +2340,7 @@
       <c r="P28"/>
       <c r="Q28"/>
       <c r="R28" s="50" t="str">
-        <f>IF(S28=$Y$5,"Rayonkampioen",IF(S28=$Y$7,"2e plaats",IF(S28=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S28" s="13">
@@ -2376,7 +2365,7 @@
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
       <c r="L29" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M29" s="21"/>
@@ -2385,7 +2374,7 @@
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29" s="50" t="str">
-        <f>IF(S29=$Y$5,"Rayonkampioen",IF(S29=$Y$7,"2e plaats",IF(S29=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S29" s="13">
@@ -2410,7 +2399,7 @@
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
       <c r="L30" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M30" s="21"/>
@@ -2419,7 +2408,7 @@
       <c r="P30"/>
       <c r="Q30"/>
       <c r="R30" s="50" t="str">
-        <f>IF(S30=$Y$5,"Rayonkampioen",IF(S30=$Y$7,"2e plaats",IF(S30=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S30" s="13">
@@ -2444,7 +2433,7 @@
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
       <c r="L31" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M31" s="21"/>
@@ -2453,7 +2442,7 @@
       <c r="P31"/>
       <c r="Q31"/>
       <c r="R31" s="50" t="str">
-        <f>IF(S31=$Y$5,"Rayonkampioen",IF(S31=$Y$7,"2e plaats",IF(S31=$Y$8,"3e plaats","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S31" s="13">
@@ -2466,27 +2455,27 @@
       <c r="W31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="56"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="69" t="str">
-        <f t="shared" ref="L32" si="2">IF(J32&lt;&gt;"",J32+K32,"")</f>
-        <v/>
-      </c>
-      <c r="M32" s="62"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="59"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="68" t="str">
+        <f t="shared" ref="L32" si="3">IF(J32&lt;&gt;"",J32+K32,"")</f>
+        <v/>
+      </c>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
       <c r="S32" s="38"/>
       <c r="T32" s="37"/>
       <c r="U32" s="37"/>
@@ -2494,22 +2483,22 @@
       <c r="W32"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="62" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="39"/>
       <c r="C33" s="38"/>
-      <c r="D33" s="64"/>
+      <c r="D33" s="63"/>
       <c r="E33" s="38"/>
       <c r="F33" s="38"/>
-      <c r="G33" s="65" t="s">
+      <c r="G33" s="64" t="s">
         <v>41</v>
       </c>
       <c r="H33" s="38"/>
-      <c r="I33" s="66"/>
+      <c r="I33" s="65"/>
       <c r="J33" s="40"/>
       <c r="K33" s="40"/>
-      <c r="L33" s="70" t="s">
+      <c r="L33" s="69" t="s">
         <v>38</v>
       </c>
       <c r="M33" s="40"/>
@@ -2517,10 +2506,10 @@
       <c r="O33" s="40"/>
       <c r="P33" s="38"/>
       <c r="Q33" s="38"/>
-      <c r="R33" s="71" t="s">
+      <c r="R33" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="S33" s="71" t="s">
+      <c r="S33" s="70" t="s">
         <v>38</v>
       </c>
       <c r="T33" s="37"/>
@@ -2529,29 +2518,29 @@
       <c r="W33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="56"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="38"/>
-      <c r="D34" s="64"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
-      <c r="G34" s="67"/>
+      <c r="G34" s="66"/>
       <c r="H34" s="38"/>
-      <c r="I34" s="66"/>
+      <c r="I34" s="65"/>
       <c r="J34" s="40"/>
       <c r="K34" s="40"/>
-      <c r="L34" s="70" t="s">
+      <c r="L34" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="72"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="71" t="s">
+      <c r="M34" s="71"/>
+      <c r="N34" s="71"/>
+      <c r="O34" s="71"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="S34" s="71" t="s">
+      <c r="S34" s="70" t="s">
         <v>38</v>
       </c>
       <c r="T34" s="37"/>
@@ -2560,29 +2549,29 @@
       <c r="W34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="62" t="s">
         <v>14</v>
       </c>
       <c r="B35" s="39"/>
       <c r="C35" s="38"/>
-      <c r="D35" s="68"/>
+      <c r="D35" s="67"/>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
-      <c r="G35" s="67"/>
+      <c r="G35" s="66"/>
       <c r="H35" s="38"/>
-      <c r="I35" s="66"/>
+      <c r="I35" s="65"/>
       <c r="J35" s="40"/>
       <c r="K35" s="40"/>
-      <c r="L35" s="78" t="s">
+      <c r="L35" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="78"/>
-      <c r="S35" s="78"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="77"/>
+      <c r="R35" s="77"/>
+      <c r="S35" s="77"/>
       <c r="T35" s="37"/>
       <c r="U35" s="37"/>
       <c r="V35"/>
@@ -2601,11 +2590,11 @@
       <c r="G36" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H36" s="77"/>
+      <c r="H36" s="76"/>
       <c r="I36" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="T36" s="77" t="s">
+      <c r="T36" s="76" t="s">
         <v>56</v>
       </c>
       <c r="U36" s="25" t="s">
@@ -2835,7 +2824,6 @@
   </sortState>
   <mergeCells count="9">
     <mergeCell ref="L35:S35"/>
-    <mergeCell ref="M3:R3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="A5:B5"/>
@@ -2843,6 +2831,7 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="S3:U3"/>
+    <mergeCell ref="J3:R3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="S7:S31">

</xml_diff>